<commit_message>
GPP vs median K & parameter table updates
</commit_message>
<xml_diff>
--- a/figures and tables/2022 Tables/Table_Parameters.xlsx
+++ b/figures and tables/2022 Tables/Table_Parameters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jblaszczak\Dropbox\UNR\Publications\2021 Productivity dynamics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jblaszczak\Documents\GitHub\RiverBiomass\figures and tables\2022 Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Symbol</t>
   </si>
@@ -42,30 +42,15 @@
     <t>Intrinsic growth rate</t>
   </si>
   <si>
-    <t>Units</t>
-  </si>
-  <si>
-    <t>day</t>
-  </si>
-  <si>
     <t>Process error</t>
   </si>
   <si>
     <t>Standard deviation of process error</t>
   </si>
   <si>
-    <t>unitless</t>
-  </si>
-  <si>
-    <t>g O2 m-2 d-1</t>
-  </si>
-  <si>
     <t>Time</t>
   </si>
   <si>
-    <t>Days</t>
-  </si>
-  <si>
     <t>$X_{t}$</t>
   </si>
   <si>
@@ -127,9 +112,6 @@
   </si>
   <si>
     <t>$B_{t}$</t>
-  </si>
-  <si>
-    <t>g C m-2 d-1</t>
   </si>
   <si>
     <t>Daily latent photosynthetically-active autotrophic biomass</t>
@@ -506,219 +488,194 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D55" sqref="A29:D55"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="24.453125" customWidth="1"/>
     <col min="2" max="2" width="55.81640625" customWidth="1"/>
-    <col min="3" max="3" width="14.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>28</v>
       </c>
       <c r="B18" t="s">
         <v>4</v>
       </c>
-      <c r="C18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
-      </c>
-      <c r="E20" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>